<commit_message>
XIRR Calculator and Metrics Comparison Dashboard complete
</commit_message>
<xml_diff>
--- a/templates/mutual-funds-holding-unit-upload-template.xlsx
+++ b/templates/mutual-funds-holding-unit-upload-template.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27425"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28324"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://onevmw-my.sharepoint.com/personal/shubhabratar_vmware_com/Documents/Rony's Files/Scaler MS Computer Science/Backend Project/Projects/MyStockPlanningApp/data-upload/templates/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://omnissa-my.sharepoint.com/personal/shubhabratar_omnissa_com/Documents/Rony's Files/Scaler MS Computer Science/Backend Project/Projects/MyStockPlanningApp/templates/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="37" documentId="8_{C6E655AB-D0D0-41DE-A7CD-BDF13AD6BBCC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{A2046AB4-6273-4446-8B40-CE901C207362}"/>
+  <xr:revisionPtr revIDLastSave="40" documentId="8_{C6E655AB-D0D0-41DE-A7CD-BDF13AD6BBCC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{3F32DA8E-CA76-411E-BF3A-13930664CDE9}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" xr2:uid="{5BCC6984-DD14-4872-863F-FC271DF83AEC}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="10">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="11">
   <si>
     <t>mutualFundInstrumentName</t>
   </si>
@@ -66,6 +66,9 @@
   </si>
   <si>
     <t>exchange_order_id</t>
+  </si>
+  <si>
+    <t>owner_name</t>
   </si>
 </sst>
 </file>
@@ -122,10 +125,6 @@
     </ext>
   </extLst>
 </styleSheet>
-</file>
-
-<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
-<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -425,72 +424,74 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{78F1ADF3-4495-4C54-BBCA-4EF0F3CC5506}">
-  <dimension ref="A1:J6"/>
+  <dimension ref="A1:K6"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B1" sqref="B1"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="3.6328125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="25.453125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="8.453125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="14.26953125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="12.26953125" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="13.54296875" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="16.36328125" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="13.90625" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="13.1796875" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="17" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="11.90625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="3.6328125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="25.453125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="8.453125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="14.26953125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="12.26953125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="13.54296875" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="16.36328125" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="13.90625" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="13.1796875" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="17" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
+        <v>10</v>
+      </c>
+      <c r="B1" t="s">
         <v>3</v>
       </c>
-      <c r="B1" t="s">
+      <c r="C1" t="s">
         <v>0</v>
       </c>
-      <c r="C1" t="s">
+      <c r="D1" t="s">
         <v>4</v>
       </c>
-      <c r="D1" t="s">
+      <c r="E1" t="s">
         <v>5</v>
       </c>
-      <c r="E1" s="2" t="s">
+      <c r="F1" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="F1" t="s">
+      <c r="G1" t="s">
         <v>2</v>
       </c>
-      <c r="G1" t="s">
+      <c r="H1" t="s">
         <v>1</v>
       </c>
-      <c r="H1" s="2" t="s">
+      <c r="I1" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="I1" s="2" t="s">
+      <c r="J1" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="J1" s="2" t="s">
+      <c r="K1" s="2" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="B2" s="1"/>
-    </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="B3" s="1"/>
-    </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="B4" s="1"/>
-    </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="B5" s="1"/>
-    </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="B6" s="1"/>
+    <row r="2" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="C2" s="1"/>
+    </row>
+    <row r="3" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="C3" s="1"/>
+    </row>
+    <row r="4" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="C4" s="1"/>
+    </row>
+    <row r="5" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="C5" s="1"/>
+    </row>
+    <row r="6" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="C6" s="1"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>